<commit_message>
revise the profit logic
</commit_message>
<xml_diff>
--- a/AMESdashboard/data/price_ratecard.xlsx
+++ b/AMESdashboard/data/price_ratecard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Albert Long\BEX5112\AMESdashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loong\Desktop\Test\bex5112\BEX5112_AMES_consulting_project\AMESdashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEE2816-6204-424E-9F0C-3EEDF53CC8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E7BC2C-8C98-47A7-BE41-C75747BB44E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sea_freight" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>POL</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>CNGZG</t>
-  </si>
-  <si>
-    <t>Express</t>
   </si>
   <si>
     <t>Normal</t>
@@ -98,6 +95,26 @@
   </si>
   <si>
     <t>Other fixed_miscellaneous</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUMEL</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>NDC sea freight</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sensitive</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>NDC Inventory</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>NDC Miscellenous</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -166,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -185,11 +202,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -203,14 +345,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,112 +670,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="33.88671875" customWidth="1"/>
+    <col min="7" max="7" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="G1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="D3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10">
+        <v>45</v>
+      </c>
+      <c r="G3" s="18">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10">
+        <v>8.5</v>
+      </c>
+      <c r="F4" s="10">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="G4" s="18">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10">
+        <v>13.5</v>
+      </c>
+      <c r="F5" s="10">
+        <v>35</v>
+      </c>
+      <c r="G5" s="18">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E6" s="10">
+        <v>6.5</v>
+      </c>
+      <c r="F6" s="10">
+        <v>30</v>
+      </c>
+      <c r="G6" s="18">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4">
+      <c r="D7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="15">
         <v>7.5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F7" s="15">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="G7" s="19">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -607,28 +867,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B36405-5386-4C6B-BA26-555904AFF2DB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="63.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="135" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="135" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
@@ -636,10 +905,16 @@
       <c r="C2" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -647,10 +922,16 @@
       <c r="C3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4">
         <v>2.5</v>
@@ -658,32 +939,50 @@
       <c r="C4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -696,7 +995,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -706,13 +1005,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -720,10 +1019,10 @@
     </row>
     <row r="2" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="C2" s="4">
         <v>10</v>
@@ -734,10 +1033,10 @@
     </row>
     <row r="3" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4">
         <v>12</v>
@@ -748,10 +1047,10 @@
     </row>
     <row r="4" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4">
         <v>15</v>

</xml_diff>